<commit_message>
Updated 6 test cases
As per changes in app, 6 test cases updated.
</commit_message>
<xml_diff>
--- a/Credentials.xlsx
+++ b/Credentials.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Email</t>
   </si>
@@ -23,18 +23,22 @@
   </si>
   <si>
     <t>test123</t>
+  </si>
+  <si>
+    <t>himanshu.sharma@diaspark.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
@@ -54,11 +58,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -289,10 +296,18 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>